<commit_message>
baru selesai, belum diuji
</commit_message>
<xml_diff>
--- a/public/format_file_upload.xlsx
+++ b/public/format_file_upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\sistem_evoting\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEE427E-39AB-424D-B47F-9D7183C89A06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CE267A-B0BB-471E-9F3E-D117ADC7F0A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{03421D34-E896-4E3C-AEC8-8704BF93EE6C}"/>
   </bookViews>
@@ -25,18 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>id_member</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>nama_member</t>
   </si>
   <si>
-    <t>isi id mulai dari baris ke 2</t>
-  </si>
-  <si>
     <t>isi nama member mulai baris ke 2</t>
+  </si>
+  <si>
+    <t>id_kta</t>
+  </si>
+  <si>
+    <t>id_ktp</t>
+  </si>
+  <si>
+    <t>isi id_ktp mulai dari baris ke 2</t>
+  </si>
+  <si>
+    <t>isi id_kta mulai dari baris ke 2</t>
   </si>
 </sst>
 </file>
@@ -402,37 +408,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C9BF275-2277-4BD1-BE04-91D6D171B589}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="2" max="2" width="34.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>